<commit_message>
UML update, guest order hotfix, edit cart items
</commit_message>
<xml_diff>
--- a/restaurantmanager/src/main/resources/Menu.xlsx
+++ b/restaurantmanager/src/main/resources/Menu.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8CED7B-EC5E-4E49-87F8-91A3F8FF4F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4125" yWindow="3390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" windowHeight="11385" windowWidth="21600" xWindow="4125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="3390"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
@@ -142,24 +142,34 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3">
     <font>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -172,15 +182,25 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -406,17 +426,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A6" workbookViewId="0" tabSelected="1">
+      <selection pane="topLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
@@ -510,7 +529,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="1">
-        <v>2.4900000000000002</v>
+        <v>2.49</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>1</v>
@@ -740,7 +759,7 @@
         <v>38</v>
       </c>
       <c r="E14" s="1">
-        <v>2.4900000000000002</v>
+        <v>2.49</v>
       </c>
       <c r="F14" s="1" t="b">
         <v>1</v>
@@ -989,7 +1008,9 @@
       <c r="C25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E25" s="1">
         <v>3.49</v>
       </c>

</xml_diff>